<commit_message>
chapter 4 discussion, summary and future directions are all filled in. Chapter 4 = "complete" (for now).
-return to evaluate Coll-OHFP with RF VIM
</commit_message>
<xml_diff>
--- a/R-inputs_UBC-forWater-MSc_HMc/tables/Workbooks/soil_analysis.xlsx
+++ b/R-inputs_UBC-forWater-MSc_HMc/tables/Workbooks/soil_analysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hannah\Documents\UBC_MSc\Thesis_UBC-forWater-MSc_HMc\R_UBC_MSc_thesis\R-inputs_UBC-forWater-MSc_HMc\tables\Workbooks_for-watershed-tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hannah\Documents\UBC_MSc\Thesis_UBC-forWater-MSc_HMc\R_UBC_MSc_thesis\R-inputs_UBC-forWater-MSc_HMc\tables\Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D9CFE7-AF7D-42C7-B854-25546C19E9D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{373DF0B1-66E0-4A73-8066-B4C715175267}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="615" windowWidth="10575" windowHeight="10260" tabRatio="855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="855" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="compilation_notes_HMc" sheetId="20" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5624" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5627" uniqueCount="244">
   <si>
     <t>SP_ID</t>
   </si>
@@ -3796,8 +3796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA64FD86-AB5F-4BAE-BE28-CCC5B6488B0E}">
   <dimension ref="A2:S39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3808,7 +3808,7 @@
     <col min="4" max="4" width="14.7109375" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.140625" customWidth="1"/>
-    <col min="7" max="7" width="48.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.7109375" customWidth="1"/>
     <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
@@ -5192,6 +5192,9 @@
         <v>212</v>
       </c>
       <c r="I33" t="s">
+        <v>240</v>
+      </c>
+      <c r="J33" t="s">
         <v>169</v>
       </c>
     </row>
@@ -5212,6 +5215,9 @@
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>54</v>
+      </c>
+      <c r="H37" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -5290,54 +5296,54 @@
       <formula>NOT(ISERROR(SEARCH("KILDONAN",A20)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I33">
+  <conditionalFormatting sqref="J33">
     <cfRule type="containsText" dxfId="280" priority="33" operator="containsText" text="BEDROCK">
-      <formula>NOT(ISERROR(SEARCH("BEDROCK",I33)))</formula>
+      <formula>NOT(ISERROR(SEARCH("BEDROCK",J33)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="279" priority="34" operator="containsText" text="CULLITE">
-      <formula>NOT(ISERROR(SEARCH("CULLITE",I33)))</formula>
+      <formula>NOT(ISERROR(SEARCH("CULLITE",J33)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="278" priority="35" operator="containsText" text="ESPINOSA">
-      <formula>NOT(ISERROR(SEARCH("ESPINOSA",I33)))</formula>
+      <formula>NOT(ISERROR(SEARCH("ESPINOSA",J33)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="277" priority="36" operator="containsText" text="ROBERTSON">
-      <formula>NOT(ISERROR(SEARCH("ROBERTSON",I33)))</formula>
+      <formula>NOT(ISERROR(SEARCH("ROBERTSON",J33)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="276" priority="37" operator="containsText" text="HONEYMOON">
-      <formula>NOT(ISERROR(SEARCH("HONEYMOON",I33)))</formula>
+      <formula>NOT(ISERROR(SEARCH("HONEYMOON",J33)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="275" priority="38" operator="containsText" text="HEALEY">
-      <formula>NOT(ISERROR(SEARCH("HEALEY",I33)))</formula>
+      <formula>NOT(ISERROR(SEARCH("HEALEY",J33)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="274" priority="39" operator="containsText" text="HERBERT">
-      <formula>NOT(ISERROR(SEARCH("HERBERT",I33)))</formula>
+      <formula>NOT(ISERROR(SEARCH("HERBERT",J33)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="273" priority="40" operator="equal">
       <formula>"PACHENA"</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="272" priority="41" operator="containsText" text="OPEN WATER">
-      <formula>NOT(ISERROR(SEARCH("OPEN WATER",I33)))</formula>
+      <formula>NOT(ISERROR(SEARCH("OPEN WATER",J33)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="271" priority="42" operator="equal">
       <formula>"ARTLISH"</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="270" priority="43" operator="containsText" text="REEGAN">
-      <formula>NOT(ISERROR(SEARCH("REEGAN",I33)))</formula>
+      <formula>NOT(ISERROR(SEARCH("REEGAN",J33)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="269" priority="44" operator="containsText" text="QUIMPER">
-      <formula>NOT(ISERROR(SEARCH("QUIMPER",I33)))</formula>
+      <formula>NOT(ISERROR(SEARCH("QUIMPER",J33)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="268" priority="45" operator="containsText" text="ZEBRIO">
-      <formula>NOT(ISERROR(SEARCH("ZEBRIO",I33)))</formula>
+      <formula>NOT(ISERROR(SEARCH("ZEBRIO",J33)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="267" priority="46" operator="containsText" text="FLEETWOOD">
-      <formula>NOT(ISERROR(SEARCH("FLEETWOOD",I33)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FLEETWOOD",J33)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="266" priority="47" operator="containsText" text="ROSSITER">
-      <formula>NOT(ISERROR(SEARCH("ROSSITER",I33)))</formula>
+      <formula>NOT(ISERROR(SEARCH("ROSSITER",J33)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="265" priority="48" operator="containsText" text="STRATA">
-      <formula>NOT(ISERROR(SEARCH("STRATA",I33)))</formula>
+      <formula>NOT(ISERROR(SEARCH("STRATA",J33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I31">
@@ -15818,7 +15824,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8AA06EC-7667-4A45-AAAD-48F5E5B25FE0}">
   <dimension ref="A1:V32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="P1" sqref="P1:V8"/>
     </sheetView>
   </sheetViews>
@@ -16540,6 +16546,9 @@
       </c>
       <c r="M13" s="14">
         <v>1.3673008513984253</v>
+      </c>
+      <c r="S13" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">

</xml_diff>